<commit_message>
Finalização do Projeto & Sprint 10
</commit_message>
<xml_diff>
--- a/Sprint-9/Product Backlog-Burndown.xlsx
+++ b/Sprint-9/Product Backlog-Burndown.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17766"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danil\Desktop\PROJETO9\adocao\Sprint-9\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danil\Desktop\Sistemas de Informação\Faculdade\PROJETO9\adocao\Sprint-9\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="185">
   <si>
     <t>Product Backlog</t>
   </si>
@@ -573,6 +573,9 @@
   </si>
   <si>
     <t>Busca e Visualização das Adoções em Tabbles</t>
+  </si>
+  <si>
+    <t>Criar classe relatorio em model</t>
   </si>
 </sst>
 </file>
@@ -945,13 +948,13 @@
     <xf numFmtId="4" fontId="13" fillId="10" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="4" fontId="7" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -963,17 +966,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -990,14 +990,11 @@
     <xf numFmtId="0" fontId="12" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1011,10 +1008,16 @@
     <xf numFmtId="164" fontId="9" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="7" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1973,10 +1976,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S119"/>
+  <dimension ref="A1:S122"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A75" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E102" sqref="E102"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A85" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F96" sqref="F96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1991,14 +1994,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -2103,10 +2106,10 @@
       <c r="S4" s="1"/>
     </row>
     <row r="5" spans="1:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="36" t="s">
         <v>53</v>
       </c>
       <c r="C5" s="21" t="s">
@@ -2136,8 +2139,8 @@
       <c r="S5" s="1"/>
     </row>
     <row r="6" spans="1:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="38"/>
-      <c r="B6" s="40"/>
+      <c r="A6" s="37"/>
+      <c r="B6" s="39"/>
       <c r="C6" s="21" t="s">
         <v>55</v>
       </c>
@@ -2165,8 +2168,8 @@
       <c r="S6" s="1"/>
     </row>
     <row r="7" spans="1:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="39"/>
-      <c r="B7" s="41"/>
+      <c r="A7" s="38"/>
+      <c r="B7" s="40"/>
       <c r="C7" s="22" t="s">
         <v>56</v>
       </c>
@@ -2430,7 +2433,7 @@
       <c r="S15" s="1"/>
     </row>
     <row r="16" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="41" t="s">
         <v>78</v>
       </c>
       <c r="B16" s="30" t="s">
@@ -2463,7 +2466,7 @@
       <c r="S16" s="1"/>
     </row>
     <row r="17" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A17" s="33"/>
+      <c r="A17" s="41"/>
       <c r="B17" s="31"/>
       <c r="C17" s="3" t="s">
         <v>59</v>
@@ -2492,7 +2495,7 @@
       <c r="S17" s="1"/>
     </row>
     <row r="18" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A18" s="33"/>
+      <c r="A18" s="41"/>
       <c r="B18" s="31"/>
       <c r="C18" s="6" t="s">
         <v>60</v>
@@ -2521,7 +2524,7 @@
       <c r="S18" s="1"/>
     </row>
     <row r="19" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A19" s="33"/>
+      <c r="A19" s="41"/>
       <c r="B19" s="31"/>
       <c r="C19" s="6" t="s">
         <v>61</v>
@@ -2550,7 +2553,7 @@
       <c r="S19" s="1"/>
     </row>
     <row r="20" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A20" s="33"/>
+      <c r="A20" s="41"/>
       <c r="B20" s="31"/>
       <c r="C20" s="6" t="s">
         <v>62</v>
@@ -2579,7 +2582,7 @@
       <c r="S20" s="1"/>
     </row>
     <row r="21" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A21" s="33"/>
+      <c r="A21" s="41"/>
       <c r="B21" s="31"/>
       <c r="C21" s="6" t="s">
         <v>63</v>
@@ -2608,7 +2611,7 @@
       <c r="S21" s="1"/>
     </row>
     <row r="22" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A22" s="33"/>
+      <c r="A22" s="41"/>
       <c r="B22" s="31"/>
       <c r="C22" s="6" t="s">
         <v>64</v>
@@ -2637,7 +2640,7 @@
       <c r="S22" s="1"/>
     </row>
     <row r="23" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A23" s="33"/>
+      <c r="A23" s="41"/>
       <c r="B23" s="31"/>
       <c r="C23" s="6" t="s">
         <v>65</v>
@@ -2666,7 +2669,7 @@
       <c r="S23" s="1"/>
     </row>
     <row r="24" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A24" s="33"/>
+      <c r="A24" s="41"/>
       <c r="B24" s="32"/>
       <c r="C24" s="4" t="s">
         <v>66</v>
@@ -3742,7 +3745,7 @@
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A78" s="27" t="s">
+      <c r="A78" s="28" t="s">
         <v>156</v>
       </c>
       <c r="B78" s="30" t="s">
@@ -3762,7 +3765,7 @@
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A79" s="28"/>
+      <c r="A79" s="29"/>
       <c r="B79" s="31"/>
       <c r="C79" s="6" t="s">
         <v>158</v>
@@ -3778,7 +3781,7 @@
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A80" s="28"/>
+      <c r="A80" s="29"/>
       <c r="B80" s="31"/>
       <c r="C80" s="6" t="s">
         <v>167</v>
@@ -3794,7 +3797,7 @@
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A81" s="28"/>
+      <c r="A81" s="29"/>
       <c r="B81" s="31"/>
       <c r="C81" s="6" t="s">
         <v>160</v>
@@ -3810,7 +3813,7 @@
       </c>
     </row>
     <row r="82" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="27" t="s">
+      <c r="A82" s="28" t="s">
         <v>159</v>
       </c>
       <c r="B82" s="30" t="s">
@@ -3830,7 +3833,7 @@
       </c>
     </row>
     <row r="83" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="28"/>
+      <c r="A83" s="29"/>
       <c r="B83" s="31"/>
       <c r="C83" s="6" t="s">
         <v>164</v>
@@ -3846,7 +3849,7 @@
       </c>
     </row>
     <row r="84" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="28"/>
+      <c r="A84" s="29"/>
       <c r="B84" s="31"/>
       <c r="C84" s="6" t="s">
         <v>165</v>
@@ -3862,7 +3865,7 @@
       </c>
     </row>
     <row r="85" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="29"/>
+      <c r="A85" s="42"/>
       <c r="B85" s="32"/>
       <c r="C85" s="6" t="s">
         <v>166</v>
@@ -3890,7 +3893,7 @@
       <c r="D86" s="5">
         <v>3</v>
       </c>
-      <c r="E86" s="50">
+      <c r="E86" s="27">
         <v>2.2999999999999998</v>
       </c>
       <c r="F86" s="6">
@@ -3906,7 +3909,7 @@
       <c r="D87" s="5">
         <v>1.5</v>
       </c>
-      <c r="E87" s="50">
+      <c r="E87" s="27">
         <v>1.85</v>
       </c>
       <c r="F87" s="6">
@@ -3922,7 +3925,7 @@
       <c r="D88" s="5">
         <v>1</v>
       </c>
-      <c r="E88" s="50">
+      <c r="E88" s="27">
         <v>0.5</v>
       </c>
       <c r="F88" s="6">
@@ -3938,7 +3941,7 @@
       <c r="D89" s="5">
         <v>1</v>
       </c>
-      <c r="E89" s="50">
+      <c r="E89" s="27">
         <v>0.25</v>
       </c>
       <c r="F89" s="6">
@@ -3954,7 +3957,7 @@
       <c r="D90" s="5">
         <v>2</v>
       </c>
-      <c r="E90" s="50">
+      <c r="E90" s="27">
         <v>1.42</v>
       </c>
       <c r="F90" s="6">
@@ -3970,7 +3973,7 @@
       <c r="D91" s="5">
         <v>5</v>
       </c>
-      <c r="E91" s="50">
+      <c r="E91" s="27">
         <v>3.75</v>
       </c>
       <c r="F91" s="6">
@@ -4033,149 +4036,155 @@
       <c r="A95" s="31"/>
       <c r="B95" s="31"/>
       <c r="C95" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="D95" s="5"/>
-      <c r="E95" s="5"/>
+        <v>182</v>
+      </c>
+      <c r="D95" s="5">
+        <v>2</v>
+      </c>
+      <c r="E95" s="5">
+        <v>1.46</v>
+      </c>
       <c r="F95" s="6">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" s="31"/>
       <c r="B96" s="31"/>
       <c r="C96" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="D96" s="5">
-        <v>2</v>
-      </c>
-      <c r="E96" s="5">
-        <v>1.46</v>
-      </c>
+        <v>184</v>
+      </c>
+      <c r="D96" s="5"/>
+      <c r="E96" s="5"/>
       <c r="F96" s="6">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A97" s="32"/>
-      <c r="B97" s="32"/>
-      <c r="C97" s="6" t="s">
-        <v>183</v>
-      </c>
+      <c r="A97" s="31"/>
+      <c r="B97" s="31"/>
+      <c r="C97" s="6"/>
       <c r="D97" s="5"/>
       <c r="E97" s="5"/>
       <c r="F97" s="6">
         <v>10</v>
       </c>
     </row>
-    <row r="98" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="25"/>
-      <c r="B98" s="25"/>
-      <c r="C98" s="25"/>
-      <c r="D98" s="26"/>
-      <c r="E98" s="26"/>
-      <c r="F98" s="25"/>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A98" s="31"/>
+      <c r="B98" s="31"/>
+      <c r="C98" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="D98" s="5"/>
+      <c r="E98" s="5"/>
+      <c r="F98" s="6">
+        <v>10</v>
+      </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A99" s="30" t="s">
-        <v>115</v>
-      </c>
-      <c r="B99" s="30" t="s">
-        <v>116</v>
-      </c>
+      <c r="A99" s="31"/>
+      <c r="B99" s="31"/>
       <c r="C99" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="D99" s="5"/>
+      <c r="E99" s="5"/>
+      <c r="F99" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A100" s="32"/>
+      <c r="B100" s="32"/>
+      <c r="C100" s="25"/>
+      <c r="D100" s="26"/>
+      <c r="E100" s="26"/>
+      <c r="F100" s="25"/>
+    </row>
+    <row r="101" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A101" s="25"/>
+      <c r="B101" s="25"/>
+      <c r="C101" s="6" t="s">
         <v>117</v>
-      </c>
-      <c r="D99" s="5">
-        <v>2</v>
-      </c>
-      <c r="E99" s="5">
-        <v>1.67</v>
-      </c>
-      <c r="F99" s="6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A100" s="31"/>
-      <c r="B100" s="31"/>
-      <c r="C100" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="D100" s="5">
-        <v>2</v>
-      </c>
-      <c r="E100" s="5">
-        <v>1.25</v>
-      </c>
-      <c r="F100" s="6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A101" s="31"/>
-      <c r="B101" s="31"/>
-      <c r="C101" s="6" t="s">
-        <v>119</v>
       </c>
       <c r="D101" s="5">
         <v>2</v>
       </c>
       <c r="E101" s="5">
-        <v>2.2000000000000002</v>
+        <v>1.67</v>
       </c>
       <c r="F101" s="6">
         <v>5</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A102" s="32"/>
-      <c r="B102" s="32"/>
+      <c r="A102" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="B102" s="30" t="s">
+        <v>116</v>
+      </c>
       <c r="C102" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D102" s="5">
         <v>2</v>
       </c>
       <c r="E102" s="5">
-        <v>2.8</v>
+        <v>1.25</v>
       </c>
       <c r="F102" s="6">
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A103" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B103" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C103" s="6"/>
-      <c r="D103" s="5"/>
-      <c r="E103" s="5"/>
-      <c r="F103" s="6"/>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A103" s="31"/>
+      <c r="B103" s="31"/>
+      <c r="C103" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D103" s="5">
+        <v>2</v>
+      </c>
+      <c r="E103" s="5">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F103" s="6">
+        <v>5</v>
+      </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A104" s="3"/>
-      <c r="B104" s="3"/>
-      <c r="C104" s="6"/>
-      <c r="D104" s="5"/>
-      <c r="E104" s="5"/>
-      <c r="F104" s="6"/>
+      <c r="A104" s="31"/>
+      <c r="B104" s="31"/>
+      <c r="C104" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D104" s="5">
+        <v>2</v>
+      </c>
+      <c r="E104" s="5">
+        <v>2.8</v>
+      </c>
+      <c r="F104" s="6">
+        <v>5</v>
+      </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A105" s="3"/>
-      <c r="B105" s="3"/>
+      <c r="A105" s="32"/>
+      <c r="B105" s="32"/>
       <c r="C105" s="6"/>
       <c r="D105" s="5"/>
       <c r="E105" s="5"/>
       <c r="F105" s="6"/>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A106" s="3"/>
-      <c r="B106" s="3"/>
+    <row r="106" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A106" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="C106" s="6"/>
       <c r="D106" s="5"/>
       <c r="E106" s="5"/>
@@ -4198,30 +4207,28 @@
       <c r="F108" s="6"/>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A109" s="6"/>
-      <c r="B109" s="6"/>
+      <c r="A109" s="3"/>
+      <c r="B109" s="3"/>
       <c r="C109" s="6"/>
       <c r="D109" s="5"/>
       <c r="E109" s="5"/>
       <c r="F109" s="6"/>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A110" s="6"/>
-      <c r="B110" s="6"/>
+      <c r="A110" s="3"/>
+      <c r="B110" s="3"/>
       <c r="C110" s="6"/>
       <c r="D110" s="5"/>
       <c r="E110" s="5"/>
       <c r="F110" s="6"/>
     </row>
-    <row r="111" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A111" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="B111" s="25"/>
-      <c r="C111" s="25"/>
-      <c r="D111" s="26"/>
-      <c r="E111" s="26"/>
-      <c r="F111" s="25"/>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A111" s="3"/>
+      <c r="B111" s="3"/>
+      <c r="C111" s="6"/>
+      <c r="D111" s="5"/>
+      <c r="E111" s="5"/>
+      <c r="F111" s="6"/>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" s="6"/>
@@ -4231,17 +4238,19 @@
       <c r="E112" s="5"/>
       <c r="F112" s="6"/>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A113" s="6"/>
       <c r="B113" s="6"/>
-      <c r="C113" s="6"/>
-      <c r="D113" s="5"/>
-      <c r="E113" s="5"/>
-      <c r="F113" s="6"/>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A114" s="6"/>
-      <c r="B114" s="6"/>
+      <c r="C113" s="25"/>
+      <c r="D113" s="26"/>
+      <c r="E113" s="26"/>
+      <c r="F113" s="25"/>
+    </row>
+    <row r="114" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A114" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B114" s="25"/>
       <c r="C114" s="6"/>
       <c r="D114" s="5"/>
       <c r="E114" s="5"/>
@@ -4264,28 +4273,77 @@
       <c r="F116" s="6"/>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A117" s="4"/>
-      <c r="B117" s="4"/>
-      <c r="C117" s="4"/>
+      <c r="A117" s="6"/>
+      <c r="B117" s="6"/>
+      <c r="C117" s="6"/>
       <c r="D117" s="5"/>
       <c r="E117" s="5"/>
       <c r="F117" s="6"/>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A118" s="4"/>
-      <c r="B118" s="4"/>
-      <c r="C118" s="7"/>
-      <c r="D118" s="8"/>
-      <c r="E118" s="8"/>
+      <c r="A118" s="6"/>
+      <c r="B118" s="6"/>
+      <c r="C118" s="6"/>
+      <c r="D118" s="5"/>
+      <c r="E118" s="5"/>
       <c r="F118" s="6"/>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A119" s="7" t="s">
+      <c r="A119" s="6"/>
+      <c r="B119" s="6"/>
+      <c r="C119" s="4"/>
+      <c r="D119" s="5"/>
+      <c r="E119" s="5"/>
+      <c r="F119" s="6"/>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A120" s="4"/>
+      <c r="B120" s="4"/>
+      <c r="C120" s="7"/>
+      <c r="D120" s="8"/>
+      <c r="E120" s="8"/>
+      <c r="F120" s="6"/>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A121" s="4"/>
+      <c r="B121" s="4"/>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A122" s="7" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="45">
+    <mergeCell ref="A102:A105"/>
+    <mergeCell ref="B102:B105"/>
+    <mergeCell ref="B86:B91"/>
+    <mergeCell ref="A86:A91"/>
+    <mergeCell ref="B92:B100"/>
+    <mergeCell ref="A92:A100"/>
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="B46:B48"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="B49:B51"/>
+    <mergeCell ref="A82:A85"/>
+    <mergeCell ref="B82:B85"/>
+    <mergeCell ref="A69:A71"/>
+    <mergeCell ref="B69:B71"/>
+    <mergeCell ref="B59:B64"/>
+    <mergeCell ref="A59:A64"/>
+    <mergeCell ref="A52:A54"/>
+    <mergeCell ref="B52:B54"/>
+    <mergeCell ref="A16:A24"/>
+    <mergeCell ref="B16:B24"/>
+    <mergeCell ref="A28:A32"/>
+    <mergeCell ref="B28:B32"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A8:A15"/>
+    <mergeCell ref="B8:B15"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B5:B7"/>
     <mergeCell ref="A78:A81"/>
     <mergeCell ref="B78:B81"/>
     <mergeCell ref="B72:B77"/>
@@ -4298,39 +4356,10 @@
     <mergeCell ref="B40:B42"/>
     <mergeCell ref="A40:A42"/>
     <mergeCell ref="B43:B45"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A8:A15"/>
-    <mergeCell ref="B8:B15"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="A16:A24"/>
-    <mergeCell ref="B16:B24"/>
-    <mergeCell ref="A28:A32"/>
-    <mergeCell ref="B28:B32"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="B25:B27"/>
     <mergeCell ref="A55:A58"/>
     <mergeCell ref="B55:B58"/>
     <mergeCell ref="A65:A68"/>
     <mergeCell ref="B65:B68"/>
-    <mergeCell ref="A69:A71"/>
-    <mergeCell ref="B69:B71"/>
-    <mergeCell ref="B59:B64"/>
-    <mergeCell ref="A59:A64"/>
-    <mergeCell ref="A52:A54"/>
-    <mergeCell ref="B52:B54"/>
-    <mergeCell ref="A46:A48"/>
-    <mergeCell ref="B46:B48"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="B49:B51"/>
-    <mergeCell ref="A82:A85"/>
-    <mergeCell ref="B82:B85"/>
-    <mergeCell ref="B92:B97"/>
-    <mergeCell ref="A92:A97"/>
-    <mergeCell ref="A99:A102"/>
-    <mergeCell ref="B99:B102"/>
-    <mergeCell ref="B86:B91"/>
-    <mergeCell ref="A86:A91"/>
   </mergeCells>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
@@ -4366,20 +4395,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="45"/>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45" t="s">
+      <c r="A1" s="43"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
       <c r="M1" s="9"/>
       <c r="N1" s="9"/>
       <c r="O1" s="1"/>
@@ -4394,40 +4423,40 @@
       <c r="X1" s="1"/>
     </row>
     <row r="2" spans="1:24" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="48" t="s">
+      <c r="C2" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="48" t="s">
+      <c r="D2" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="48" t="s">
+      <c r="E2" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="42" t="s">
+      <c r="F2" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="49" t="s">
+      <c r="G2" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="49" t="s">
+      <c r="H2" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="42" t="s">
+      <c r="I2" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="42" t="s">
+      <c r="J2" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="42" t="s">
+      <c r="K2" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="42" t="s">
+      <c r="L2" s="47" t="s">
         <v>22</v>
       </c>
       <c r="O2" s="1"/>
@@ -4442,18 +4471,18 @@
       <c r="X2" s="1"/>
     </row>
     <row r="3" spans="1:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="46"/>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="49"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
-      <c r="K3" s="42"/>
-      <c r="L3" s="42"/>
+      <c r="A3" s="44"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="47"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
@@ -4641,22 +4670,22 @@
       <c r="X7" s="1"/>
     </row>
     <row r="8" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="43" t="s">
+      <c r="A8" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="43"/>
-      <c r="C8" s="43" t="s">
+      <c r="B8" s="49"/>
+      <c r="C8" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="43"/>
-      <c r="I8" s="43"/>
-      <c r="J8" s="43"/>
-      <c r="K8" s="43"/>
-      <c r="L8" s="43"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="49"/>
+      <c r="H8" s="49"/>
+      <c r="I8" s="49"/>
+      <c r="J8" s="49"/>
+      <c r="K8" s="49"/>
+      <c r="L8" s="49"/>
       <c r="M8" s="17" t="s">
         <v>9</v>
       </c>
@@ -4675,10 +4704,10 @@
       <c r="X8" s="1"/>
     </row>
     <row r="9" spans="1:24" ht="18" x14ac:dyDescent="0.2">
-      <c r="A9" s="44">
+      <c r="A9" s="50">
         <v>50</v>
       </c>
-      <c r="B9" s="44"/>
+      <c r="B9" s="50"/>
       <c r="C9" s="15">
         <f>SUMIF('Product Backlog'!F:F,1,'Product Backlog'!E:E)</f>
         <v>35</v>
@@ -4740,6 +4769,9 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:L8"/>
+    <mergeCell ref="A9:B9"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:L1"/>
     <mergeCell ref="A2:A3"/>
@@ -4754,9 +4786,6 @@
     <mergeCell ref="J2:J3"/>
     <mergeCell ref="K2:K3"/>
     <mergeCell ref="L2:L3"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:L8"/>
-    <mergeCell ref="A9:B9"/>
   </mergeCells>
   <conditionalFormatting sqref="C10:N91">
     <cfRule type="expression" dxfId="2" priority="2">

</xml_diff>